<commit_message>
Excel Datei Reiter Linien ergänzt
</commit_message>
<xml_diff>
--- a/DiTWP_212-UE_Punkte.xlsx
+++ b/DiTWP_212-UE_Punkte.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ARI\41_FH_Wien\DiTWP\212_UE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ARI\41_FH_Wien\DiTWP\311_VO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{690B4604-26D0-4882-95D3-38BCB13847AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1592EEAC-5643-43C8-ACA7-BBE52A394E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12015" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QS" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Linie" sheetId="3" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -360,7 +361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6C8634-08D4-4DB6-B767-A65A626282F8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -383,6 +384,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBBDF35-882C-4C5D-8DD2-A95ACC6225BD}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>